<commit_message>
debtrank implementated. Missing adjustments in capital buffer and investments parameters
</commit_message>
<xml_diff>
--- a/adj_matrix.xlsx
+++ b/adj_matrix.xlsx
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>185.3901149227057</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -553,7 +553,7 @@
         <v>0</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <v>187.9884851080575</v>
       </c>
       <c r="AE2">
         <v>0</v>
@@ -576,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>95.94689056523418</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -585,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>10.32331763302869</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -609,13 +609,13 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>28.28668428403349</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3">
-        <v>13.04889315425236</v>
+        <v>150.1310015817778</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -627,7 +627,7 @@
         <v>0</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>196.8604391758524</v>
       </c>
       <c r="X3">
         <v>0</v>
@@ -639,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="AA3">
-        <v>84.64874268331843</v>
+        <v>0</v>
       </c>
       <c r="AB3">
         <v>0</v>
@@ -674,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1.111717471350082</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>34.24347347326133</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>0</v>
+        <v>167.775720771107</v>
       </c>
       <c r="AC4">
         <v>0</v>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>49.40431712919045</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -775,7 +775,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>63.9079653857624</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -784,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>46.28321089717047</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -793,7 +793,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>33.18147658491325</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -802,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>167.9153402463508</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -826,7 +826,7 @@
         <v>0</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>100.7553394673655</v>
       </c>
       <c r="AA5">
         <v>0</v>
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>49.00208262751264</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -873,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>181.5221913118031</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -891,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>55.60119156374645</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -903,10 +903,10 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>193.0410977412918</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>152.856166140868</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -918,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="Y6">
-        <v>0</v>
+        <v>159.6626230917951</v>
       </c>
       <c r="Z6">
         <v>0</v>
@@ -927,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="AB6">
-        <v>0</v>
+        <v>46.56762015541631</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -962,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>7.275451017233925</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -974,13 +974,13 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>80.65947074088903</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>43.56036642424102</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -992,16 +992,16 @@
         <v>0</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>76.94643731847638</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>119.2290395715406</v>
       </c>
       <c r="T7">
         <v>0</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>132.5830079260408</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>29.9136160948252</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1069,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>62.69152010808789</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>69.9595483632778</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -1105,16 +1105,16 @@
         <v>0</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <v>60.69780122155435</v>
       </c>
       <c r="Y8">
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <v>150.0011984146961</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <v>40.15186014115548</v>
       </c>
       <c r="AB8">
         <v>0</v>
@@ -1209,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="AA9">
-        <v>50.09807491806314</v>
+        <v>0</v>
       </c>
       <c r="AB9">
         <v>0</v>
@@ -1232,13 +1232,13 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>75.4351757400276</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>61.61995085843572</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1271,7 +1271,7 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>66.38174720444958</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -1286,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>146.9720258416792</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -1298,13 +1298,13 @@
         <v>0</v>
       </c>
       <c r="Y10">
-        <v>0</v>
+        <v>122.7429672168996</v>
       </c>
       <c r="Z10">
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>0</v>
+        <v>192.0267570975421</v>
       </c>
       <c r="AB10">
         <v>0</v>
@@ -1327,7 +1327,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>131.7461276268717</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1345,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>98.06645730313166</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1354,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>27.86354882950966</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1375,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>59.8127427345013</v>
       </c>
       <c r="T11">
         <v>0</v>
@@ -1384,7 +1384,7 @@
         <v>0</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>140.5124702930762</v>
       </c>
       <c r="W11">
         <v>0</v>
@@ -1399,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>135.2030467813716</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -1408,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="AD11">
-        <v>87.10263190779858</v>
+        <v>0</v>
       </c>
       <c r="AE11">
         <v>0</v>
@@ -1428,10 +1428,10 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>56.71581912830517</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>186.9376378245593</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1452,13 +1452,13 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>90.3770029481288</v>
+        <v>0</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
-        <v>26.92206138331812</v>
+        <v>0</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1470,13 +1470,13 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>28.81411903578286</v>
+        <v>122.2396488798556</v>
       </c>
       <c r="T12">
         <v>0</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>50.8611802002809</v>
       </c>
       <c r="V12">
         <v>0</v>
@@ -1488,10 +1488,10 @@
         <v>0</v>
       </c>
       <c r="Y12">
-        <v>0</v>
+        <v>114.9802407312519</v>
       </c>
       <c r="Z12">
-        <v>43.37504221907879</v>
+        <v>0</v>
       </c>
       <c r="AA12">
         <v>0</v>
@@ -1514,7 +1514,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>60.57730256776104</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1580,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>55.67383796497867</v>
       </c>
       <c r="Y13">
         <v>0</v>
@@ -1595,13 +1595,13 @@
         <v>0</v>
       </c>
       <c r="AC13">
-        <v>0</v>
+        <v>133.8674284005627</v>
       </c>
       <c r="AD13">
-        <v>31.57712127688057</v>
+        <v>0</v>
       </c>
       <c r="AE13">
-        <v>0</v>
+        <v>139.5846115125957</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -1618,10 +1618,10 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>119.9388001706701</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>176.1177051987486</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1633,7 +1633,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>192.5400163637157</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1642,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>64.79984791280602</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -1657,7 +1657,7 @@
         <v>0</v>
       </c>
       <c r="R14">
-        <v>34.30093568180118</v>
+        <v>0</v>
       </c>
       <c r="S14">
         <v>0</v>
@@ -1678,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="Y14">
-        <v>65.79441290720189</v>
+        <v>0</v>
       </c>
       <c r="Z14">
         <v>0</v>
@@ -1693,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="AD14">
-        <v>0</v>
+        <v>147.2582676252367</v>
       </c>
       <c r="AE14">
         <v>0</v>
@@ -1728,13 +1728,13 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>23.12706909340125</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>59.13755813526858</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>63.63715947293589</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1770,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>75.8584487278179</v>
       </c>
       <c r="Y15">
         <v>0</v>
@@ -1799,7 +1799,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>35.94990851071083</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1817,7 +1817,7 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>173.7089986416413</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1826,7 +1826,7 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>22.2359132871029</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -1844,10 +1844,10 @@
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>40.78577126878217</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>92.91983231216105</v>
+        <v>0</v>
       </c>
       <c r="S16">
         <v>0</v>
@@ -1862,10 +1862,10 @@
         <v>0</v>
       </c>
       <c r="W16">
-        <v>60.93322180595362</v>
+        <v>0</v>
       </c>
       <c r="X16">
-        <v>69.72281249573774</v>
+        <v>0</v>
       </c>
       <c r="Y16">
         <v>0</v>
@@ -1874,7 +1874,7 @@
         <v>0</v>
       </c>
       <c r="AA16">
-        <v>70.81228603308482</v>
+        <v>0</v>
       </c>
       <c r="AB16">
         <v>0</v>
@@ -1897,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>76.43114366501406</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>77.00258026144473</v>
+        <v>181.050703490946</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1927,13 +1927,13 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>6.595724476533271</v>
+        <v>0</v>
       </c>
       <c r="N17">
         <v>0</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>191.1339795008002</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -1942,10 +1942,10 @@
         <v>0</v>
       </c>
       <c r="R17">
-        <v>70.54224612559975</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>11.71405332298782</v>
+        <v>0</v>
       </c>
       <c r="T17">
         <v>0</v>
@@ -1954,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="V17">
-        <v>71.33145847195216</v>
+        <v>0</v>
       </c>
       <c r="W17">
         <v>0</v>
@@ -1992,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>13.15959474207462</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2013,10 +2013,10 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>27.67436238789873</v>
       </c>
       <c r="K18">
-        <v>76.81343396738794</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -2064,7 +2064,7 @@
         <v>0</v>
       </c>
       <c r="AA18">
-        <v>63.77442713885804</v>
+        <v>3.477124494654427</v>
       </c>
       <c r="AB18">
         <v>0</v>
@@ -2084,7 +2084,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>48.96766975713056</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2105,13 +2105,13 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>135.3966807924818</v>
       </c>
       <c r="J19">
-        <v>25.96702550208261</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>58.97598601450174</v>
+        <v>0</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -2144,16 +2144,16 @@
         <v>0</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>141.5892427938283</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>98.49183067922618</v>
       </c>
       <c r="X19">
         <v>0</v>
       </c>
       <c r="Y19">
-        <v>0</v>
+        <v>144.8837424607011</v>
       </c>
       <c r="Z19">
         <v>0</v>
@@ -2182,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>83.05115025630701</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2194,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>59.50936990817479</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -2212,10 +2212,10 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>5.810390817416455</v>
       </c>
       <c r="N20">
-        <v>71.78870337571473</v>
+        <v>0</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -2227,7 +2227,7 @@
         <v>0</v>
       </c>
       <c r="R20">
-        <v>34.53062791681249</v>
+        <v>0</v>
       </c>
       <c r="S20">
         <v>0</v>
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="V20">
-        <v>78.74395265403582</v>
+        <v>0</v>
       </c>
       <c r="W20">
         <v>0</v>
@@ -2251,10 +2251,10 @@
         <v>0</v>
       </c>
       <c r="Z20">
-        <v>1.31690673626883</v>
+        <v>0</v>
       </c>
       <c r="AA20">
-        <v>0</v>
+        <v>164.1831165485813</v>
       </c>
       <c r="AB20">
         <v>0</v>
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="AD20">
-        <v>0</v>
+        <v>109.8081415153659</v>
       </c>
       <c r="AE20">
         <v>0</v>
@@ -2313,7 +2313,7 @@
         <v>0</v>
       </c>
       <c r="O21">
-        <v>1.232569542309414</v>
+        <v>113.817046644803</v>
       </c>
       <c r="P21">
         <v>0</v>
@@ -2325,7 +2325,7 @@
         <v>0</v>
       </c>
       <c r="S21">
-        <v>15.37773235643051</v>
+        <v>0</v>
       </c>
       <c r="T21">
         <v>0</v>
@@ -2340,7 +2340,7 @@
         <v>0</v>
       </c>
       <c r="X21">
-        <v>18.18270820633756</v>
+        <v>0</v>
       </c>
       <c r="Y21">
         <v>0</v>
@@ -2349,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="AA21">
-        <v>65.01365091256004</v>
+        <v>0</v>
       </c>
       <c r="AB21">
         <v>0</v>
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>73.98213654092689</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -2414,7 +2414,7 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>0.3050613965543514</v>
       </c>
       <c r="R22">
         <v>0</v>
@@ -2441,10 +2441,10 @@
         <v>0</v>
       </c>
       <c r="Z22">
-        <v>0</v>
+        <v>159.9123534890697</v>
       </c>
       <c r="AA22">
-        <v>86.09538972171434</v>
+        <v>0</v>
       </c>
       <c r="AB22">
         <v>0</v>
@@ -2456,7 +2456,7 @@
         <v>0</v>
       </c>
       <c r="AE22">
-        <v>0</v>
+        <v>105.4185342872002</v>
       </c>
     </row>
     <row r="23" spans="1:31">
@@ -2473,7 +2473,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>13.30285461636986</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2506,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>181.1219945622685</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="X23">
-        <v>0</v>
+        <v>55.14463800256786</v>
       </c>
       <c r="Y23">
         <v>0</v>
@@ -2580,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>79.30013583558666</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -2619,7 +2619,7 @@
         <v>0</v>
       </c>
       <c r="V24">
-        <v>0</v>
+        <v>188.174734618735</v>
       </c>
       <c r="W24">
         <v>0</v>
@@ -2640,13 +2640,13 @@
         <v>0</v>
       </c>
       <c r="AC24">
-        <v>0</v>
+        <v>12.22364148619475</v>
       </c>
       <c r="AD24">
         <v>0</v>
       </c>
       <c r="AE24">
-        <v>62.55367842872278</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:31">
@@ -2654,7 +2654,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>9.511300515692845</v>
+        <v>0</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2708,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="T25">
-        <v>0</v>
+        <v>107.2530760813871</v>
       </c>
       <c r="U25">
         <v>0</v>
@@ -2758,25 +2758,25 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>99.98449429737997</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
-        <v>53.45866241101598</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>57.31051449563687</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>48.55913634208196</v>
+        <v>0</v>
       </c>
       <c r="J26">
         <v>0</v>
       </c>
       <c r="K26">
-        <v>67.53112198379834</v>
+        <v>102.9108913985278</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -2809,7 +2809,7 @@
         <v>0</v>
       </c>
       <c r="V26">
-        <v>6.662968605507502</v>
+        <v>36.79175731258779</v>
       </c>
       <c r="W26">
         <v>0</v>
@@ -2836,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="AE26">
-        <v>0</v>
+        <v>41.7294991912611</v>
       </c>
     </row>
     <row r="27" spans="1:31">
@@ -2844,7 +2844,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>55.25864131291704</v>
+        <v>0</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -2865,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>162.7638769258638</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -2889,7 +2889,7 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>99.87579238868545</v>
+        <v>0</v>
       </c>
       <c r="R27">
         <v>0</v>
@@ -2922,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="AB27">
-        <v>19.60315817408847</v>
+        <v>93.60126849868251</v>
       </c>
       <c r="AC27">
         <v>0</v>
@@ -2939,7 +2939,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>49.2782099872956</v>
+        <v>131.6757503849493</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2969,7 +2969,7 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>160.6846614163516</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -3011,7 +3011,7 @@
         <v>0</v>
       </c>
       <c r="Z28">
-        <v>0</v>
+        <v>6.152500669787653</v>
       </c>
       <c r="AA28">
         <v>0</v>
@@ -3040,10 +3040,10 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>92.33045406461052</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>97.225033004919</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -3058,7 +3058,7 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>45.32619768342816</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -3082,13 +3082,13 @@
         <v>0</v>
       </c>
       <c r="R29">
-        <v>35.03268702034836</v>
+        <v>0</v>
       </c>
       <c r="S29">
         <v>0</v>
       </c>
       <c r="T29">
-        <v>0</v>
+        <v>54.69283743325095</v>
       </c>
       <c r="U29">
         <v>0</v>
@@ -3106,7 +3106,7 @@
         <v>0</v>
       </c>
       <c r="Z29">
-        <v>75.36734043761014</v>
+        <v>0</v>
       </c>
       <c r="AA29">
         <v>0</v>
@@ -3118,7 +3118,7 @@
         <v>0</v>
       </c>
       <c r="AD29">
-        <v>0</v>
+        <v>151.3117526103657</v>
       </c>
       <c r="AE29">
         <v>0</v>
@@ -3171,7 +3171,7 @@
         <v>0</v>
       </c>
       <c r="P30">
-        <v>0</v>
+        <v>127.7914282145141</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -3186,7 +3186,7 @@
         <v>0</v>
       </c>
       <c r="U30">
-        <v>0</v>
+        <v>49.65861353749552</v>
       </c>
       <c r="V30">
         <v>0</v>
@@ -3198,10 +3198,10 @@
         <v>0</v>
       </c>
       <c r="Y30">
-        <v>0</v>
+        <v>109.8278416991078</v>
       </c>
       <c r="Z30">
-        <v>26.5467225580617</v>
+        <v>0</v>
       </c>
       <c r="AA30">
         <v>0</v>
@@ -3233,7 +3233,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>61.00932928235871</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -3242,7 +3242,7 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>127.1312804989518</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -3269,10 +3269,10 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>0</v>
+        <v>150.7790807799552</v>
       </c>
       <c r="R31">
-        <v>0</v>
+        <v>43.32180468213116</v>
       </c>
       <c r="S31">
         <v>0</v>
@@ -3293,7 +3293,7 @@
         <v>0</v>
       </c>
       <c r="Y31">
-        <v>3.231895062179191</v>
+        <v>0</v>
       </c>
       <c r="Z31">
         <v>0</v>
@@ -3305,7 +3305,7 @@
         <v>0</v>
       </c>
       <c r="AC31">
-        <v>0</v>
+        <v>42.05273010064246</v>
       </c>
       <c r="AD31">
         <v>0</v>

</xml_diff>